<commit_message>
Einbindung von WP2 und WP5 in byLocations
</commit_message>
<xml_diff>
--- a/_uniform_words.xlsx
+++ b/_uniform_words.xlsx
@@ -182,7 +182,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="678" uniqueCount="281">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="679" uniqueCount="281">
   <si>
     <t>byFunctions</t>
   </si>
@@ -4669,9 +4669,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L334"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A88" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K102" sqref="K102"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A25" sqref="A25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5673,9 +5673,8 @@
       </c>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A24" t="str">
-        <f>IF($E24&lt;&gt;"","-","")</f>
-        <v>-</v>
+      <c r="A24" t="s">
+        <v>228</v>
       </c>
       <c r="B24" t="s">
         <v>218</v>

</xml_diff>